<commit_message>
all files generated from model runs
</commit_message>
<xml_diff>
--- a/models/calculation engines/economic_overlay/outputs/CBIX_BX_AA_production_cost.xlsx
+++ b/models/calculation engines/economic_overlay/outputs/CBIX_BX_AA_production_cost.xlsx
@@ -533,10 +533,10 @@
         <v>1085.185185185185</v>
       </c>
       <c r="F3" t="n">
-        <v>515.3674944444444</v>
+        <v>515.3679148061111</v>
       </c>
       <c r="G3" t="n">
-        <v>407.2192635739547</v>
+        <v>407.2193467859372</v>
       </c>
       <c r="H3" t="n">
         <v>9.359999999999999</v>
@@ -548,7 +548,7 @@
         <v>305</v>
       </c>
       <c r="K3" t="n">
-        <v>2358.45937530235</v>
+        <v>2358.459878875999</v>
       </c>
     </row>
     <row r="4">
@@ -563,7 +563,7 @@
       <c r="I4" t="inlineStr"/>
       <c r="J4" t="inlineStr"/>
       <c r="K4" t="n">
-        <v>2358.45937530235</v>
+        <v>2358.459878875999</v>
       </c>
     </row>
     <row r="5">
@@ -578,7 +578,7 @@
       <c r="I5" t="inlineStr"/>
       <c r="J5" t="inlineStr"/>
       <c r="K5" t="n">
-        <v>2358.45937530235</v>
+        <v>2358.459878875999</v>
       </c>
     </row>
     <row r="6">
@@ -593,7 +593,7 @@
       <c r="I6" t="inlineStr"/>
       <c r="J6" t="inlineStr"/>
       <c r="K6" t="n">
-        <v>2358.45937530235</v>
+        <v>2358.459878875999</v>
       </c>
     </row>
     <row r="7">
@@ -608,7 +608,7 @@
       <c r="I7" t="inlineStr"/>
       <c r="J7" t="inlineStr"/>
       <c r="K7" t="n">
-        <v>2358.45937530235</v>
+        <v>2358.459878875999</v>
       </c>
     </row>
     <row r="8">
@@ -623,7 +623,7 @@
       <c r="I8" t="inlineStr"/>
       <c r="J8" t="inlineStr"/>
       <c r="K8" t="n">
-        <v>2358.45937530235</v>
+        <v>2358.459878875999</v>
       </c>
     </row>
     <row r="9">
@@ -638,7 +638,7 @@
       <c r="I9" t="inlineStr"/>
       <c r="J9" t="inlineStr"/>
       <c r="K9" t="n">
-        <v>2358.45937530235</v>
+        <v>2358.459878875999</v>
       </c>
     </row>
     <row r="10">
@@ -653,7 +653,7 @@
       <c r="I10" t="inlineStr"/>
       <c r="J10" t="inlineStr"/>
       <c r="K10" t="n">
-        <v>2358.45937530235</v>
+        <v>2358.459878875999</v>
       </c>
     </row>
     <row r="11">
@@ -668,7 +668,7 @@
       <c r="I11" t="inlineStr"/>
       <c r="J11" t="inlineStr"/>
       <c r="K11" t="n">
-        <v>2358.45937530235</v>
+        <v>2358.459878875999</v>
       </c>
     </row>
     <row r="12">
@@ -683,7 +683,7 @@
       <c r="I12" t="inlineStr"/>
       <c r="J12" t="inlineStr"/>
       <c r="K12" t="n">
-        <v>2358.45937530235</v>
+        <v>2358.459878875999</v>
       </c>
     </row>
     <row r="13">
@@ -698,7 +698,7 @@
       <c r="I13" t="inlineStr"/>
       <c r="J13" t="inlineStr"/>
       <c r="K13" t="n">
-        <v>2358.45937530235</v>
+        <v>2358.459878875999</v>
       </c>
     </row>
     <row r="14">
@@ -713,7 +713,7 @@
       <c r="I14" t="inlineStr"/>
       <c r="J14" t="inlineStr"/>
       <c r="K14" t="n">
-        <v>2358.45937530235</v>
+        <v>2358.459878875999</v>
       </c>
     </row>
     <row r="15">
@@ -728,7 +728,7 @@
       <c r="I15" t="inlineStr"/>
       <c r="J15" t="inlineStr"/>
       <c r="K15" t="n">
-        <v>2358.45937530235</v>
+        <v>2358.459878875999</v>
       </c>
     </row>
     <row r="16">
@@ -743,7 +743,7 @@
       <c r="I16" t="inlineStr"/>
       <c r="J16" t="inlineStr"/>
       <c r="K16" t="n">
-        <v>2358.45937530235</v>
+        <v>2358.459878875999</v>
       </c>
     </row>
     <row r="17">
@@ -758,7 +758,7 @@
       <c r="I17" t="inlineStr"/>
       <c r="J17" t="inlineStr"/>
       <c r="K17" t="n">
-        <v>2358.45937530235</v>
+        <v>2358.459878875999</v>
       </c>
     </row>
     <row r="18">
@@ -773,7 +773,7 @@
       <c r="I18" t="inlineStr"/>
       <c r="J18" t="inlineStr"/>
       <c r="K18" t="n">
-        <v>2358.45937530235</v>
+        <v>2358.459878875999</v>
       </c>
     </row>
     <row r="19">
@@ -788,7 +788,7 @@
       <c r="I19" t="inlineStr"/>
       <c r="J19" t="inlineStr"/>
       <c r="K19" t="n">
-        <v>2358.45937530235</v>
+        <v>2358.459878875999</v>
       </c>
     </row>
     <row r="20">
@@ -803,7 +803,7 @@
       <c r="I20" t="inlineStr"/>
       <c r="J20" t="inlineStr"/>
       <c r="K20" t="n">
-        <v>2358.45937530235</v>
+        <v>2358.459878875999</v>
       </c>
     </row>
     <row r="21">
@@ -818,7 +818,7 @@
       <c r="I21" t="inlineStr"/>
       <c r="J21" t="inlineStr"/>
       <c r="K21" t="n">
-        <v>2358.45937530235</v>
+        <v>2358.459878875999</v>
       </c>
     </row>
     <row r="22">
@@ -833,7 +833,7 @@
       <c r="I22" t="inlineStr"/>
       <c r="J22" t="inlineStr"/>
       <c r="K22" t="n">
-        <v>2358.45937530235</v>
+        <v>2358.459878875999</v>
       </c>
     </row>
     <row r="23">
@@ -848,7 +848,7 @@
       <c r="I23" t="inlineStr"/>
       <c r="J23" t="inlineStr"/>
       <c r="K23" t="n">
-        <v>2358.45937530235</v>
+        <v>2358.459878875999</v>
       </c>
     </row>
     <row r="24">
@@ -863,7 +863,7 @@
       <c r="I24" t="inlineStr"/>
       <c r="J24" t="inlineStr"/>
       <c r="K24" t="n">
-        <v>2358.45937530235</v>
+        <v>2358.459878875999</v>
       </c>
     </row>
     <row r="25">
@@ -878,7 +878,7 @@
       <c r="I25" t="inlineStr"/>
       <c r="J25" t="inlineStr"/>
       <c r="K25" t="n">
-        <v>2358.45937530235</v>
+        <v>2358.459878875999</v>
       </c>
     </row>
     <row r="26">
@@ -893,7 +893,7 @@
       <c r="I26" t="inlineStr"/>
       <c r="J26" t="inlineStr"/>
       <c r="K26" t="n">
-        <v>2358.45937530235</v>
+        <v>2358.459878875999</v>
       </c>
     </row>
     <row r="27">
@@ -908,7 +908,7 @@
       <c r="I27" t="inlineStr"/>
       <c r="J27" t="inlineStr"/>
       <c r="K27" t="n">
-        <v>2358.45937530235</v>
+        <v>2358.459878875999</v>
       </c>
     </row>
     <row r="28">
@@ -923,7 +923,7 @@
       <c r="I28" t="inlineStr"/>
       <c r="J28" t="inlineStr"/>
       <c r="K28" t="n">
-        <v>2358.45937530235</v>
+        <v>2358.459878875999</v>
       </c>
     </row>
     <row r="29">
@@ -938,7 +938,7 @@
       <c r="I29" t="inlineStr"/>
       <c r="J29" t="inlineStr"/>
       <c r="K29" t="n">
-        <v>2358.45937530235</v>
+        <v>2358.459878875999</v>
       </c>
     </row>
     <row r="30">
@@ -953,7 +953,7 @@
       <c r="I30" t="inlineStr"/>
       <c r="J30" t="inlineStr"/>
       <c r="K30" t="n">
-        <v>2358.45937530235</v>
+        <v>2358.459878875999</v>
       </c>
     </row>
     <row r="31">
@@ -968,7 +968,7 @@
       <c r="I31" t="inlineStr"/>
       <c r="J31" t="inlineStr"/>
       <c r="K31" t="n">
-        <v>2358.45937530235</v>
+        <v>2358.459878875999</v>
       </c>
     </row>
     <row r="32">
@@ -983,7 +983,7 @@
       <c r="I32" t="inlineStr"/>
       <c r="J32" t="inlineStr"/>
       <c r="K32" t="n">
-        <v>2358.45937530235</v>
+        <v>2358.459878875999</v>
       </c>
     </row>
     <row r="33">
@@ -998,7 +998,7 @@
       <c r="I33" t="inlineStr"/>
       <c r="J33" t="inlineStr"/>
       <c r="K33" t="n">
-        <v>2358.45937530235</v>
+        <v>2358.459878875999</v>
       </c>
     </row>
     <row r="34">
@@ -1013,7 +1013,7 @@
       <c r="I34" t="inlineStr"/>
       <c r="J34" t="inlineStr"/>
       <c r="K34" t="n">
-        <v>2358.45937530235</v>
+        <v>2358.459878875999</v>
       </c>
     </row>
     <row r="35">
@@ -1028,7 +1028,7 @@
       <c r="I35" t="inlineStr"/>
       <c r="J35" t="inlineStr"/>
       <c r="K35" t="n">
-        <v>2358.45937530235</v>
+        <v>2358.459878875999</v>
       </c>
     </row>
     <row r="36">
@@ -1043,7 +1043,7 @@
       <c r="I36" t="inlineStr"/>
       <c r="J36" t="inlineStr"/>
       <c r="K36" t="n">
-        <v>2358.45937530235</v>
+        <v>2358.459878875999</v>
       </c>
     </row>
     <row r="37">
@@ -1058,7 +1058,7 @@
       <c r="I37" t="inlineStr"/>
       <c r="J37" t="inlineStr"/>
       <c r="K37" t="n">
-        <v>2358.45937530235</v>
+        <v>2358.459878875999</v>
       </c>
     </row>
     <row r="38">
@@ -1073,7 +1073,7 @@
       <c r="I38" t="inlineStr"/>
       <c r="J38" t="inlineStr"/>
       <c r="K38" t="n">
-        <v>2358.45937530235</v>
+        <v>2358.459878875999</v>
       </c>
     </row>
     <row r="39">
@@ -1088,7 +1088,7 @@
       <c r="I39" t="inlineStr"/>
       <c r="J39" t="inlineStr"/>
       <c r="K39" t="n">
-        <v>2358.45937530235</v>
+        <v>2358.459878875999</v>
       </c>
     </row>
     <row r="40">
@@ -1103,7 +1103,7 @@
       <c r="I40" t="inlineStr"/>
       <c r="J40" t="inlineStr"/>
       <c r="K40" t="n">
-        <v>2358.45937530235</v>
+        <v>2358.459878875999</v>
       </c>
     </row>
     <row r="41">
@@ -1118,7 +1118,7 @@
       <c r="I41" t="inlineStr"/>
       <c r="J41" t="inlineStr"/>
       <c r="K41" t="n">
-        <v>2358.45937530235</v>
+        <v>2358.459878875999</v>
       </c>
     </row>
     <row r="42">
@@ -1133,7 +1133,7 @@
       <c r="I42" t="inlineStr"/>
       <c r="J42" t="inlineStr"/>
       <c r="K42" t="n">
-        <v>2358.45937530235</v>
+        <v>2358.459878875999</v>
       </c>
     </row>
     <row r="43">
@@ -1148,7 +1148,7 @@
       <c r="I43" t="inlineStr"/>
       <c r="J43" t="inlineStr"/>
       <c r="K43" t="n">
-        <v>2358.45937530235</v>
+        <v>2358.459878875999</v>
       </c>
     </row>
     <row r="44">
@@ -1163,7 +1163,7 @@
       <c r="I44" t="inlineStr"/>
       <c r="J44" t="inlineStr"/>
       <c r="K44" t="n">
-        <v>2358.45937530235</v>
+        <v>2358.459878875999</v>
       </c>
     </row>
     <row r="45">
@@ -1178,7 +1178,7 @@
       <c r="I45" t="inlineStr"/>
       <c r="J45" t="inlineStr"/>
       <c r="K45" t="n">
-        <v>2358.45937530235</v>
+        <v>2358.459878875999</v>
       </c>
     </row>
     <row r="46">
@@ -1193,7 +1193,7 @@
       <c r="I46" t="inlineStr"/>
       <c r="J46" t="inlineStr"/>
       <c r="K46" t="n">
-        <v>2358.45937530235</v>
+        <v>2358.459878875999</v>
       </c>
     </row>
     <row r="47">
@@ -1208,7 +1208,7 @@
       <c r="I47" t="inlineStr"/>
       <c r="J47" t="inlineStr"/>
       <c r="K47" t="n">
-        <v>2358.45937530235</v>
+        <v>2358.459878875999</v>
       </c>
     </row>
     <row r="48">
@@ -1223,7 +1223,7 @@
       <c r="I48" t="inlineStr"/>
       <c r="J48" t="inlineStr"/>
       <c r="K48" t="n">
-        <v>2358.45937530235</v>
+        <v>2358.459878875999</v>
       </c>
     </row>
     <row r="49">
@@ -1238,7 +1238,7 @@
       <c r="I49" t="inlineStr"/>
       <c r="J49" t="inlineStr"/>
       <c r="K49" t="n">
-        <v>2358.45937530235</v>
+        <v>2358.459878875999</v>
       </c>
     </row>
     <row r="50">
@@ -1253,7 +1253,7 @@
       <c r="I50" t="inlineStr"/>
       <c r="J50" t="inlineStr"/>
       <c r="K50" t="n">
-        <v>2358.45937530235</v>
+        <v>2358.459878875999</v>
       </c>
     </row>
     <row r="51">
@@ -1268,7 +1268,7 @@
       <c r="I51" t="inlineStr"/>
       <c r="J51" t="inlineStr"/>
       <c r="K51" t="n">
-        <v>2358.45937530235</v>
+        <v>2358.459878875999</v>
       </c>
     </row>
     <row r="52">
@@ -1283,7 +1283,7 @@
       <c r="I52" t="inlineStr"/>
       <c r="J52" t="inlineStr"/>
       <c r="K52" t="n">
-        <v>2358.45937530235</v>
+        <v>2358.459878875999</v>
       </c>
     </row>
     <row r="53">
@@ -1298,7 +1298,7 @@
       <c r="I53" t="inlineStr"/>
       <c r="J53" t="inlineStr"/>
       <c r="K53" t="n">
-        <v>2358.45937530235</v>
+        <v>2358.459878875999</v>
       </c>
     </row>
     <row r="54">
@@ -1313,7 +1313,7 @@
       <c r="I54" t="inlineStr"/>
       <c r="J54" t="inlineStr"/>
       <c r="K54" t="n">
-        <v>2358.45937530235</v>
+        <v>2358.459878875999</v>
       </c>
     </row>
     <row r="55">
@@ -1328,7 +1328,7 @@
       <c r="I55" t="inlineStr"/>
       <c r="J55" t="inlineStr"/>
       <c r="K55" t="n">
-        <v>2358.45937530235</v>
+        <v>2358.459878875999</v>
       </c>
     </row>
     <row r="56">
@@ -1343,7 +1343,7 @@
       <c r="I56" t="inlineStr"/>
       <c r="J56" t="inlineStr"/>
       <c r="K56" t="n">
-        <v>2358.45937530235</v>
+        <v>2358.459878875999</v>
       </c>
     </row>
     <row r="57">
@@ -1358,7 +1358,7 @@
       <c r="I57" t="inlineStr"/>
       <c r="J57" t="inlineStr"/>
       <c r="K57" t="n">
-        <v>2358.45937530235</v>
+        <v>2358.459878875999</v>
       </c>
     </row>
     <row r="58">
@@ -1373,7 +1373,7 @@
       <c r="I58" t="inlineStr"/>
       <c r="J58" t="inlineStr"/>
       <c r="K58" t="n">
-        <v>2358.45937530235</v>
+        <v>2358.459878875999</v>
       </c>
     </row>
     <row r="59">
@@ -1388,7 +1388,7 @@
       <c r="I59" t="inlineStr"/>
       <c r="J59" t="inlineStr"/>
       <c r="K59" t="n">
-        <v>2358.45937530235</v>
+        <v>2358.459878875999</v>
       </c>
     </row>
     <row r="60">
@@ -1403,7 +1403,7 @@
       <c r="I60" t="inlineStr"/>
       <c r="J60" t="inlineStr"/>
       <c r="K60" t="n">
-        <v>2358.45937530235</v>
+        <v>2358.459878875999</v>
       </c>
     </row>
     <row r="61">
@@ -1418,7 +1418,7 @@
       <c r="I61" t="inlineStr"/>
       <c r="J61" t="inlineStr"/>
       <c r="K61" t="n">
-        <v>2358.45937530235</v>
+        <v>2358.459878875999</v>
       </c>
     </row>
     <row r="62">
@@ -1433,7 +1433,7 @@
       <c r="I62" t="inlineStr"/>
       <c r="J62" t="inlineStr"/>
       <c r="K62" t="n">
-        <v>2358.45937530235</v>
+        <v>2358.459878875999</v>
       </c>
     </row>
     <row r="63">
@@ -1448,7 +1448,7 @@
       <c r="I63" t="inlineStr"/>
       <c r="J63" t="inlineStr"/>
       <c r="K63" t="n">
-        <v>2358.45937530235</v>
+        <v>2358.459878875999</v>
       </c>
     </row>
     <row r="64">
@@ -1463,7 +1463,7 @@
       <c r="I64" t="inlineStr"/>
       <c r="J64" t="inlineStr"/>
       <c r="K64" t="n">
-        <v>2358.45937530235</v>
+        <v>2358.459878875999</v>
       </c>
     </row>
     <row r="65">
@@ -1478,7 +1478,7 @@
       <c r="I65" t="inlineStr"/>
       <c r="J65" t="inlineStr"/>
       <c r="K65" t="n">
-        <v>2358.45937530235</v>
+        <v>2358.459878875999</v>
       </c>
     </row>
     <row r="66">
@@ -1493,7 +1493,7 @@
       <c r="I66" t="inlineStr"/>
       <c r="J66" t="inlineStr"/>
       <c r="K66" t="n">
-        <v>2358.45937530235</v>
+        <v>2358.459878875999</v>
       </c>
     </row>
     <row r="67">
@@ -1508,7 +1508,7 @@
       <c r="I67" t="inlineStr"/>
       <c r="J67" t="inlineStr"/>
       <c r="K67" t="n">
-        <v>2358.45937530235</v>
+        <v>2358.459878875999</v>
       </c>
     </row>
     <row r="68">
@@ -1523,7 +1523,7 @@
       <c r="I68" t="inlineStr"/>
       <c r="J68" t="inlineStr"/>
       <c r="K68" t="n">
-        <v>2358.45937530235</v>
+        <v>2358.459878875999</v>
       </c>
     </row>
     <row r="69">
@@ -1538,7 +1538,7 @@
       <c r="I69" t="inlineStr"/>
       <c r="J69" t="inlineStr"/>
       <c r="K69" t="n">
-        <v>2358.45937530235</v>
+        <v>2358.459878875999</v>
       </c>
     </row>
     <row r="70">
@@ -1553,7 +1553,7 @@
       <c r="I70" t="inlineStr"/>
       <c r="J70" t="inlineStr"/>
       <c r="K70" t="n">
-        <v>2358.45937530235</v>
+        <v>2358.459878875999</v>
       </c>
     </row>
     <row r="71">
@@ -1568,7 +1568,7 @@
       <c r="I71" t="inlineStr"/>
       <c r="J71" t="inlineStr"/>
       <c r="K71" t="n">
-        <v>2358.45937530235</v>
+        <v>2358.459878875999</v>
       </c>
     </row>
     <row r="72">
@@ -1583,7 +1583,7 @@
       <c r="I72" t="inlineStr"/>
       <c r="J72" t="inlineStr"/>
       <c r="K72" t="n">
-        <v>2358.45937530235</v>
+        <v>2358.459878875999</v>
       </c>
     </row>
     <row r="73">
@@ -1598,7 +1598,7 @@
       <c r="I73" t="inlineStr"/>
       <c r="J73" t="inlineStr"/>
       <c r="K73" t="n">
-        <v>2358.45937530235</v>
+        <v>2358.459878875999</v>
       </c>
     </row>
     <row r="74">
@@ -1613,7 +1613,7 @@
       <c r="I74" t="inlineStr"/>
       <c r="J74" t="inlineStr"/>
       <c r="K74" t="n">
-        <v>2358.45937530235</v>
+        <v>2358.459878875999</v>
       </c>
     </row>
     <row r="75">
@@ -1628,7 +1628,7 @@
       <c r="I75" t="inlineStr"/>
       <c r="J75" t="inlineStr"/>
       <c r="K75" t="n">
-        <v>2358.45937530235</v>
+        <v>2358.459878875999</v>
       </c>
     </row>
     <row r="76">
@@ -1643,7 +1643,7 @@
       <c r="I76" t="inlineStr"/>
       <c r="J76" t="inlineStr"/>
       <c r="K76" t="n">
-        <v>2358.45937530235</v>
+        <v>2358.459878875999</v>
       </c>
     </row>
     <row r="77">
@@ -1658,7 +1658,7 @@
       <c r="I77" t="inlineStr"/>
       <c r="J77" t="inlineStr"/>
       <c r="K77" t="n">
-        <v>2358.45937530235</v>
+        <v>2358.459878875999</v>
       </c>
     </row>
     <row r="78">
@@ -1673,7 +1673,7 @@
       <c r="I78" t="inlineStr"/>
       <c r="J78" t="inlineStr"/>
       <c r="K78" t="n">
-        <v>2358.45937530235</v>
+        <v>2358.459878875999</v>
       </c>
     </row>
     <row r="79">
@@ -1688,7 +1688,7 @@
       <c r="I79" t="inlineStr"/>
       <c r="J79" t="inlineStr"/>
       <c r="K79" t="n">
-        <v>2358.45937530235</v>
+        <v>2358.459878875999</v>
       </c>
     </row>
     <row r="80">
@@ -1703,7 +1703,7 @@
       <c r="I80" t="inlineStr"/>
       <c r="J80" t="inlineStr"/>
       <c r="K80" t="n">
-        <v>2358.45937530235</v>
+        <v>2358.459878875999</v>
       </c>
     </row>
     <row r="81">
@@ -1718,7 +1718,7 @@
       <c r="I81" t="inlineStr"/>
       <c r="J81" t="inlineStr"/>
       <c r="K81" t="n">
-        <v>2358.45937530235</v>
+        <v>2358.459878875999</v>
       </c>
     </row>
     <row r="82">
@@ -1733,7 +1733,7 @@
       <c r="I82" t="inlineStr"/>
       <c r="J82" t="inlineStr"/>
       <c r="K82" t="n">
-        <v>2358.45937530235</v>
+        <v>2358.459878875999</v>
       </c>
     </row>
     <row r="83">
@@ -1748,7 +1748,7 @@
       <c r="I83" t="inlineStr"/>
       <c r="J83" t="inlineStr"/>
       <c r="K83" t="n">
-        <v>2358.45937530235</v>
+        <v>2358.459878875999</v>
       </c>
     </row>
     <row r="84">
@@ -1763,7 +1763,7 @@
       <c r="I84" t="inlineStr"/>
       <c r="J84" t="inlineStr"/>
       <c r="K84" t="n">
-        <v>2358.45937530235</v>
+        <v>2358.459878875999</v>
       </c>
     </row>
     <row r="85">
@@ -1778,7 +1778,7 @@
       <c r="I85" t="inlineStr"/>
       <c r="J85" t="inlineStr"/>
       <c r="K85" t="n">
-        <v>2358.45937530235</v>
+        <v>2358.459878875999</v>
       </c>
     </row>
     <row r="86">
@@ -1793,7 +1793,7 @@
       <c r="I86" t="inlineStr"/>
       <c r="J86" t="inlineStr"/>
       <c r="K86" t="n">
-        <v>2358.45937530235</v>
+        <v>2358.459878875999</v>
       </c>
     </row>
     <row r="87">
@@ -1808,7 +1808,7 @@
       <c r="I87" t="inlineStr"/>
       <c r="J87" t="inlineStr"/>
       <c r="K87" t="n">
-        <v>2358.45937530235</v>
+        <v>2358.459878875999</v>
       </c>
     </row>
     <row r="88">
@@ -1823,7 +1823,7 @@
       <c r="I88" t="inlineStr"/>
       <c r="J88" t="inlineStr"/>
       <c r="K88" t="n">
-        <v>2358.45937530235</v>
+        <v>2358.459878875999</v>
       </c>
     </row>
     <row r="89">
@@ -1838,7 +1838,7 @@
       <c r="I89" t="inlineStr"/>
       <c r="J89" t="inlineStr"/>
       <c r="K89" t="n">
-        <v>2358.45937530235</v>
+        <v>2358.459878875999</v>
       </c>
     </row>
     <row r="90">
@@ -1853,7 +1853,7 @@
       <c r="I90" t="inlineStr"/>
       <c r="J90" t="inlineStr"/>
       <c r="K90" t="n">
-        <v>2358.45937530235</v>
+        <v>2358.459878875999</v>
       </c>
     </row>
     <row r="91">
@@ -1868,7 +1868,7 @@
       <c r="I91" t="inlineStr"/>
       <c r="J91" t="inlineStr"/>
       <c r="K91" t="n">
-        <v>2358.45937530235</v>
+        <v>2358.459878875999</v>
       </c>
     </row>
     <row r="92">
@@ -1883,7 +1883,7 @@
       <c r="I92" t="inlineStr"/>
       <c r="J92" t="inlineStr"/>
       <c r="K92" t="n">
-        <v>2358.45937530235</v>
+        <v>2358.459878875999</v>
       </c>
     </row>
     <row r="93">
@@ -1898,7 +1898,7 @@
       <c r="I93" t="inlineStr"/>
       <c r="J93" t="inlineStr"/>
       <c r="K93" t="n">
-        <v>2358.45937530235</v>
+        <v>2358.459878875999</v>
       </c>
     </row>
     <row r="94">
@@ -1913,7 +1913,7 @@
       <c r="I94" t="inlineStr"/>
       <c r="J94" t="inlineStr"/>
       <c r="K94" t="n">
-        <v>2358.45937530235</v>
+        <v>2358.459878875999</v>
       </c>
     </row>
     <row r="95">
@@ -1928,7 +1928,7 @@
       <c r="I95" t="inlineStr"/>
       <c r="J95" t="inlineStr"/>
       <c r="K95" t="n">
-        <v>2358.45937530235</v>
+        <v>2358.459878875999</v>
       </c>
     </row>
     <row r="96">
@@ -1943,7 +1943,7 @@
       <c r="I96" t="inlineStr"/>
       <c r="J96" t="inlineStr"/>
       <c r="K96" t="n">
-        <v>2358.45937530235</v>
+        <v>2358.459878875999</v>
       </c>
     </row>
     <row r="97">
@@ -1958,7 +1958,7 @@
       <c r="I97" t="inlineStr"/>
       <c r="J97" t="inlineStr"/>
       <c r="K97" t="n">
-        <v>2358.45937530235</v>
+        <v>2358.459878875999</v>
       </c>
     </row>
     <row r="98">
@@ -1973,7 +1973,7 @@
       <c r="I98" t="inlineStr"/>
       <c r="J98" t="inlineStr"/>
       <c r="K98" t="n">
-        <v>2358.45937530235</v>
+        <v>2358.459878875999</v>
       </c>
     </row>
     <row r="99">
@@ -1988,7 +1988,7 @@
       <c r="I99" t="inlineStr"/>
       <c r="J99" t="inlineStr"/>
       <c r="K99" t="n">
-        <v>2358.45937530235</v>
+        <v>2358.459878875999</v>
       </c>
     </row>
     <row r="100">
@@ -2003,7 +2003,7 @@
       <c r="I100" t="inlineStr"/>
       <c r="J100" t="inlineStr"/>
       <c r="K100" t="n">
-        <v>2358.45937530235</v>
+        <v>2358.459878875999</v>
       </c>
     </row>
     <row r="101">
@@ -2018,7 +2018,7 @@
       <c r="I101" t="inlineStr"/>
       <c r="J101" t="inlineStr"/>
       <c r="K101" t="n">
-        <v>2358.45937530235</v>
+        <v>2358.459878875999</v>
       </c>
     </row>
     <row r="102">
@@ -2033,7 +2033,7 @@
       <c r="I102" t="inlineStr"/>
       <c r="J102" t="inlineStr"/>
       <c r="K102" t="n">
-        <v>2358.45937530235</v>
+        <v>2358.459878875999</v>
       </c>
     </row>
     <row r="103">
@@ -2048,7 +2048,7 @@
       <c r="I103" t="inlineStr"/>
       <c r="J103" t="inlineStr"/>
       <c r="K103" t="n">
-        <v>2358.45937530235</v>
+        <v>2358.459878875999</v>
       </c>
     </row>
     <row r="104">
@@ -2063,7 +2063,7 @@
       <c r="I104" t="inlineStr"/>
       <c r="J104" t="inlineStr"/>
       <c r="K104" t="n">
-        <v>2358.45937530235</v>
+        <v>2358.459878875999</v>
       </c>
     </row>
     <row r="105">
@@ -2078,7 +2078,7 @@
       <c r="I105" t="inlineStr"/>
       <c r="J105" t="inlineStr"/>
       <c r="K105" t="n">
-        <v>2358.45937530235</v>
+        <v>2358.459878875999</v>
       </c>
     </row>
     <row r="106">
@@ -2093,7 +2093,7 @@
       <c r="I106" t="inlineStr"/>
       <c r="J106" t="inlineStr"/>
       <c r="K106" t="n">
-        <v>2358.45937530235</v>
+        <v>2358.459878875999</v>
       </c>
     </row>
     <row r="107">
@@ -2108,7 +2108,7 @@
       <c r="I107" t="inlineStr"/>
       <c r="J107" t="inlineStr"/>
       <c r="K107" t="n">
-        <v>2358.45937530235</v>
+        <v>2358.459878875999</v>
       </c>
     </row>
     <row r="108">
@@ -2123,7 +2123,7 @@
       <c r="I108" t="inlineStr"/>
       <c r="J108" t="inlineStr"/>
       <c r="K108" t="n">
-        <v>2358.45937530235</v>
+        <v>2358.459878875999</v>
       </c>
     </row>
     <row r="109">
@@ -2138,7 +2138,7 @@
       <c r="I109" t="inlineStr"/>
       <c r="J109" t="inlineStr"/>
       <c r="K109" t="n">
-        <v>2358.45937530235</v>
+        <v>2358.459878875999</v>
       </c>
     </row>
     <row r="110">
@@ -2153,7 +2153,7 @@
       <c r="I110" t="inlineStr"/>
       <c r="J110" t="inlineStr"/>
       <c r="K110" t="n">
-        <v>2358.45937530235</v>
+        <v>2358.459878875999</v>
       </c>
     </row>
     <row r="111">
@@ -2168,7 +2168,7 @@
       <c r="I111" t="inlineStr"/>
       <c r="J111" t="inlineStr"/>
       <c r="K111" t="n">
-        <v>2358.45937530235</v>
+        <v>2358.459878875999</v>
       </c>
     </row>
     <row r="112">
@@ -2183,7 +2183,7 @@
       <c r="I112" t="inlineStr"/>
       <c r="J112" t="inlineStr"/>
       <c r="K112" t="n">
-        <v>2358.45937530235</v>
+        <v>2358.459878875999</v>
       </c>
     </row>
     <row r="113">
@@ -2198,7 +2198,7 @@
       <c r="I113" t="inlineStr"/>
       <c r="J113" t="inlineStr"/>
       <c r="K113" t="n">
-        <v>2358.45937530235</v>
+        <v>2358.459878875999</v>
       </c>
     </row>
     <row r="114">
@@ -2213,7 +2213,7 @@
       <c r="I114" t="inlineStr"/>
       <c r="J114" t="inlineStr"/>
       <c r="K114" t="n">
-        <v>2358.45937530235</v>
+        <v>2358.459878875999</v>
       </c>
     </row>
     <row r="115">
@@ -2228,7 +2228,7 @@
       <c r="I115" t="inlineStr"/>
       <c r="J115" t="inlineStr"/>
       <c r="K115" t="n">
-        <v>2358.45937530235</v>
+        <v>2358.459878875999</v>
       </c>
     </row>
     <row r="116">
@@ -2243,7 +2243,7 @@
       <c r="I116" t="inlineStr"/>
       <c r="J116" t="inlineStr"/>
       <c r="K116" t="n">
-        <v>2358.45937530235</v>
+        <v>2358.459878875999</v>
       </c>
     </row>
     <row r="117">
@@ -2258,7 +2258,7 @@
       <c r="I117" t="inlineStr"/>
       <c r="J117" t="inlineStr"/>
       <c r="K117" t="n">
-        <v>2358.45937530235</v>
+        <v>2358.459878875999</v>
       </c>
     </row>
     <row r="118">
@@ -2273,7 +2273,7 @@
       <c r="I118" t="inlineStr"/>
       <c r="J118" t="inlineStr"/>
       <c r="K118" t="n">
-        <v>2358.45937530235</v>
+        <v>2358.459878875999</v>
       </c>
     </row>
     <row r="119">
@@ -2288,7 +2288,7 @@
       <c r="I119" t="inlineStr"/>
       <c r="J119" t="inlineStr"/>
       <c r="K119" t="n">
-        <v>2358.45937530235</v>
+        <v>2358.459878875999</v>
       </c>
     </row>
     <row r="120">
@@ -2303,7 +2303,7 @@
       <c r="I120" t="inlineStr"/>
       <c r="J120" t="inlineStr"/>
       <c r="K120" t="n">
-        <v>2358.45937530235</v>
+        <v>2358.459878875999</v>
       </c>
     </row>
     <row r="121">
@@ -2318,7 +2318,7 @@
       <c r="I121" t="inlineStr"/>
       <c r="J121" t="inlineStr"/>
       <c r="K121" t="n">
-        <v>2358.45937530235</v>
+        <v>2358.459878875999</v>
       </c>
     </row>
     <row r="122">
@@ -2333,7 +2333,7 @@
       <c r="I122" t="inlineStr"/>
       <c r="J122" t="inlineStr"/>
       <c r="K122" t="n">
-        <v>2358.45937530235</v>
+        <v>2358.459878875999</v>
       </c>
     </row>
     <row r="123">
@@ -2348,7 +2348,7 @@
       <c r="I123" t="inlineStr"/>
       <c r="J123" t="inlineStr"/>
       <c r="K123" t="n">
-        <v>2358.45937530235</v>
+        <v>2358.459878875999</v>
       </c>
     </row>
     <row r="124">
@@ -2363,7 +2363,7 @@
       <c r="I124" t="inlineStr"/>
       <c r="J124" t="inlineStr"/>
       <c r="K124" t="n">
-        <v>2358.45937530235</v>
+        <v>2358.459878875999</v>
       </c>
     </row>
     <row r="125">
@@ -2378,7 +2378,7 @@
       <c r="I125" t="inlineStr"/>
       <c r="J125" t="inlineStr"/>
       <c r="K125" t="n">
-        <v>2358.45937530235</v>
+        <v>2358.459878875999</v>
       </c>
     </row>
     <row r="126">
@@ -2393,7 +2393,7 @@
       <c r="I126" t="inlineStr"/>
       <c r="J126" t="inlineStr"/>
       <c r="K126" t="n">
-        <v>2358.45937530235</v>
+        <v>2358.459878875999</v>
       </c>
     </row>
     <row r="127">
@@ -2408,7 +2408,7 @@
       <c r="I127" t="inlineStr"/>
       <c r="J127" t="inlineStr"/>
       <c r="K127" t="n">
-        <v>2358.45937530235</v>
+        <v>2358.459878875999</v>
       </c>
     </row>
     <row r="128">
@@ -2423,7 +2423,7 @@
       <c r="I128" t="inlineStr"/>
       <c r="J128" t="inlineStr"/>
       <c r="K128" t="n">
-        <v>2358.45937530235</v>
+        <v>2358.459878875999</v>
       </c>
     </row>
     <row r="129">
@@ -2438,7 +2438,7 @@
       <c r="I129" t="inlineStr"/>
       <c r="J129" t="inlineStr"/>
       <c r="K129" t="n">
-        <v>2358.45937530235</v>
+        <v>2358.459878875999</v>
       </c>
     </row>
     <row r="130">
@@ -2453,7 +2453,7 @@
       <c r="I130" t="inlineStr"/>
       <c r="J130" t="inlineStr"/>
       <c r="K130" t="n">
-        <v>2358.45937530235</v>
+        <v>2358.459878875999</v>
       </c>
     </row>
     <row r="131">
@@ -2468,7 +2468,7 @@
       <c r="I131" t="inlineStr"/>
       <c r="J131" t="inlineStr"/>
       <c r="K131" t="n">
-        <v>2358.45937530235</v>
+        <v>2358.459878875999</v>
       </c>
     </row>
     <row r="132">
@@ -2483,7 +2483,7 @@
       <c r="I132" t="inlineStr"/>
       <c r="J132" t="inlineStr"/>
       <c r="K132" t="n">
-        <v>2358.45937530235</v>
+        <v>2358.459878875999</v>
       </c>
     </row>
     <row r="133">
@@ -2498,7 +2498,7 @@
       <c r="I133" t="inlineStr"/>
       <c r="J133" t="inlineStr"/>
       <c r="K133" t="n">
-        <v>2358.45937530235</v>
+        <v>2358.459878875999</v>
       </c>
     </row>
     <row r="134">
@@ -2513,7 +2513,7 @@
       <c r="I134" t="inlineStr"/>
       <c r="J134" t="inlineStr"/>
       <c r="K134" t="n">
-        <v>2358.45937530235</v>
+        <v>2358.459878875999</v>
       </c>
     </row>
     <row r="135">
@@ -2528,7 +2528,7 @@
       <c r="I135" t="inlineStr"/>
       <c r="J135" t="inlineStr"/>
       <c r="K135" t="n">
-        <v>2358.45937530235</v>
+        <v>2358.459878875999</v>
       </c>
     </row>
     <row r="136">
@@ -2543,7 +2543,7 @@
       <c r="I136" t="inlineStr"/>
       <c r="J136" t="inlineStr"/>
       <c r="K136" t="n">
-        <v>2358.45937530235</v>
+        <v>2358.459878875999</v>
       </c>
     </row>
     <row r="137">
@@ -2558,7 +2558,7 @@
       <c r="I137" t="inlineStr"/>
       <c r="J137" t="inlineStr"/>
       <c r="K137" t="n">
-        <v>2358.45937530235</v>
+        <v>2358.459878875999</v>
       </c>
     </row>
     <row r="138">
@@ -2573,7 +2573,7 @@
       <c r="I138" t="inlineStr"/>
       <c r="J138" t="inlineStr"/>
       <c r="K138" t="n">
-        <v>2358.45937530235</v>
+        <v>2358.459878875999</v>
       </c>
     </row>
     <row r="139">
@@ -2588,7 +2588,7 @@
       <c r="I139" t="inlineStr"/>
       <c r="J139" t="inlineStr"/>
       <c r="K139" t="n">
-        <v>2358.45937530235</v>
+        <v>2358.459878875999</v>
       </c>
     </row>
     <row r="140">
@@ -2603,7 +2603,7 @@
       <c r="I140" t="inlineStr"/>
       <c r="J140" t="inlineStr"/>
       <c r="K140" t="n">
-        <v>2358.45937530235</v>
+        <v>2358.459878875999</v>
       </c>
     </row>
     <row r="141">
@@ -2618,7 +2618,7 @@
       <c r="I141" t="inlineStr"/>
       <c r="J141" t="inlineStr"/>
       <c r="K141" t="n">
-        <v>2358.45937530235</v>
+        <v>2358.459878875999</v>
       </c>
     </row>
     <row r="142">
@@ -2633,7 +2633,7 @@
       <c r="I142" t="inlineStr"/>
       <c r="J142" t="inlineStr"/>
       <c r="K142" t="n">
-        <v>2358.45937530235</v>
+        <v>2358.459878875999</v>
       </c>
     </row>
     <row r="143">
@@ -2648,7 +2648,7 @@
       <c r="I143" t="inlineStr"/>
       <c r="J143" t="inlineStr"/>
       <c r="K143" t="n">
-        <v>2358.45937530235</v>
+        <v>2358.459878875999</v>
       </c>
     </row>
     <row r="144">
@@ -2663,7 +2663,7 @@
       <c r="I144" t="inlineStr"/>
       <c r="J144" t="inlineStr"/>
       <c r="K144" t="n">
-        <v>2358.45937530235</v>
+        <v>2358.459878875999</v>
       </c>
     </row>
     <row r="145">
@@ -2678,7 +2678,7 @@
       <c r="I145" t="inlineStr"/>
       <c r="J145" t="inlineStr"/>
       <c r="K145" t="n">
-        <v>2358.45937530235</v>
+        <v>2358.459878875999</v>
       </c>
     </row>
     <row r="146">
@@ -2693,7 +2693,7 @@
       <c r="I146" t="inlineStr"/>
       <c r="J146" t="inlineStr"/>
       <c r="K146" t="n">
-        <v>2358.45937530235</v>
+        <v>2358.459878875999</v>
       </c>
     </row>
     <row r="147">
@@ -2708,7 +2708,7 @@
       <c r="I147" t="inlineStr"/>
       <c r="J147" t="inlineStr"/>
       <c r="K147" t="n">
-        <v>2358.45937530235</v>
+        <v>2358.459878875999</v>
       </c>
     </row>
     <row r="148">
@@ -2723,7 +2723,7 @@
       <c r="I148" t="inlineStr"/>
       <c r="J148" t="inlineStr"/>
       <c r="K148" t="n">
-        <v>2358.45937530235</v>
+        <v>2358.459878875999</v>
       </c>
     </row>
     <row r="149">
@@ -2738,7 +2738,7 @@
       <c r="I149" t="inlineStr"/>
       <c r="J149" t="inlineStr"/>
       <c r="K149" t="n">
-        <v>2358.45937530235</v>
+        <v>2358.459878875999</v>
       </c>
     </row>
     <row r="150">
@@ -2753,7 +2753,7 @@
       <c r="I150" t="inlineStr"/>
       <c r="J150" t="inlineStr"/>
       <c r="K150" t="n">
-        <v>2358.45937530235</v>
+        <v>2358.459878875999</v>
       </c>
     </row>
     <row r="151">
@@ -2768,7 +2768,7 @@
       <c r="I151" t="inlineStr"/>
       <c r="J151" t="inlineStr"/>
       <c r="K151" t="n">
-        <v>2358.45937530235</v>
+        <v>2358.459878875999</v>
       </c>
     </row>
     <row r="152">
@@ -2783,7 +2783,7 @@
       <c r="I152" t="inlineStr"/>
       <c r="J152" t="inlineStr"/>
       <c r="K152" t="n">
-        <v>2358.45937530235</v>
+        <v>2358.459878875999</v>
       </c>
     </row>
     <row r="153">
@@ -2798,7 +2798,7 @@
       <c r="I153" t="inlineStr"/>
       <c r="J153" t="inlineStr"/>
       <c r="K153" t="n">
-        <v>2358.45937530235</v>
+        <v>2358.459878875999</v>
       </c>
     </row>
     <row r="154">
@@ -2813,7 +2813,7 @@
       <c r="I154" t="inlineStr"/>
       <c r="J154" t="inlineStr"/>
       <c r="K154" t="n">
-        <v>2358.45937530235</v>
+        <v>2358.459878875999</v>
       </c>
     </row>
     <row r="155">
@@ -2828,7 +2828,7 @@
       <c r="I155" t="inlineStr"/>
       <c r="J155" t="inlineStr"/>
       <c r="K155" t="n">
-        <v>2358.45937530235</v>
+        <v>2358.459878875999</v>
       </c>
     </row>
     <row r="156">
@@ -2843,7 +2843,7 @@
       <c r="I156" t="inlineStr"/>
       <c r="J156" t="inlineStr"/>
       <c r="K156" t="n">
-        <v>2358.45937530235</v>
+        <v>2358.459878875999</v>
       </c>
     </row>
     <row r="157">
@@ -2858,7 +2858,7 @@
       <c r="I157" t="inlineStr"/>
       <c r="J157" t="inlineStr"/>
       <c r="K157" t="n">
-        <v>2358.45937530235</v>
+        <v>2358.459878875999</v>
       </c>
     </row>
     <row r="158">
@@ -2873,7 +2873,7 @@
       <c r="I158" t="inlineStr"/>
       <c r="J158" t="inlineStr"/>
       <c r="K158" t="n">
-        <v>2358.45937530235</v>
+        <v>2358.459878875999</v>
       </c>
     </row>
     <row r="159">
@@ -2888,7 +2888,7 @@
       <c r="I159" t="inlineStr"/>
       <c r="J159" t="inlineStr"/>
       <c r="K159" t="n">
-        <v>2358.45937530235</v>
+        <v>2358.459878875999</v>
       </c>
     </row>
     <row r="160">
@@ -2903,7 +2903,7 @@
       <c r="I160" t="inlineStr"/>
       <c r="J160" t="inlineStr"/>
       <c r="K160" t="n">
-        <v>2358.45937530235</v>
+        <v>2358.459878875999</v>
       </c>
     </row>
     <row r="161">
@@ -2918,7 +2918,7 @@
       <c r="I161" t="inlineStr"/>
       <c r="J161" t="inlineStr"/>
       <c r="K161" t="n">
-        <v>2358.45937530235</v>
+        <v>2358.459878875999</v>
       </c>
     </row>
     <row r="162">
@@ -2933,7 +2933,7 @@
       <c r="I162" t="inlineStr"/>
       <c r="J162" t="inlineStr"/>
       <c r="K162" t="n">
-        <v>2358.45937530235</v>
+        <v>2358.459878875999</v>
       </c>
     </row>
     <row r="163">
@@ -2948,7 +2948,7 @@
       <c r="I163" t="inlineStr"/>
       <c r="J163" t="inlineStr"/>
       <c r="K163" t="n">
-        <v>2358.45937530235</v>
+        <v>2358.459878875999</v>
       </c>
     </row>
     <row r="164">
@@ -2963,7 +2963,7 @@
       <c r="I164" t="inlineStr"/>
       <c r="J164" t="inlineStr"/>
       <c r="K164" t="n">
-        <v>2358.45937530235</v>
+        <v>2358.459878875999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>